<commit_message>
update fsh version and add antlr4 to devDeps 5f97fc8e7567dba4d30cd10e7513a712b35b593c
</commit_message>
<xml_diff>
--- a/ig/ft/#3-add-narative/StructureDefinition-cds-fr-related-person.xlsx
+++ b/ig/ft/#3-add-narative/StructureDefinition-cds-fr-related-person.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-05T12:43:33+00:00</t>
+    <t>2023-08-23T13:14:09+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -136,6 +136,10 @@
     <t>Information about a person that is involved in the care for a patient, but who is not the target of healthcare, nor has a formal responsibility in the care process.</t>
   </si>
   <si>
+    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}</t>
+  </si>
+  <si>
     <t>role</t>
   </si>
   <si>
@@ -337,7 +341,7 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -1073,7 +1077,7 @@
     <t>An address expressed using postal conventions (as opposed to GPS or other location definition formats).  This data type may be used to convey addresses for use in delivering mail as well as for visiting locations which might not be valid for mail delivery.  There are a variety of postal address formats defined around the world.</t>
   </si>
   <si>
-    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](location.html#) resource).</t>
+    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
   </si>
   <si>
     <t>Need to keep track where the related person can be contacted per postal mail or visited.</t>
@@ -1121,10 +1125,6 @@
   </si>
   <si>
     <t>The period of time during which this relationship is or was active. If there are no dates defined, then the interval is unknown.</t>
-  </si>
-  <si>
-    <t>A Period specifies a range of time; the context of use will specify whether the entire range applies (e.g. "the patient was an inpatient of the hospital for this time range") or one value from the range applies (e.g. "give to the patient between these two times").
-Period is not used for a duration (a measure of elapsed time). See [Duration](datatypes.html#Duration).</t>
   </si>
   <si>
     <t>.effectiveTime</t>
@@ -1658,10 +1658,10 @@
         <v>34</v>
       </c>
       <c r="AJ1" t="s" s="2">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="AK1" t="s" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AL1" t="s" s="2">
         <v>34</v>
@@ -1672,10 +1672,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" t="s" s="2">
@@ -1686,7 +1686,7 @@
         <v>35</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s" s="2">
         <v>34</v>
@@ -1695,19 +1695,19 @@
         <v>34</v>
       </c>
       <c r="J2" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s" s="2">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N2" t="s" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O2" s="2"/>
       <c r="P2" t="s" s="2">
@@ -1757,13 +1757,13 @@
         <v>34</v>
       </c>
       <c r="AF2" t="s" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AG2" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH2" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI2" t="s" s="2">
         <v>34</v>
@@ -1783,10 +1783,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s" s="2">
@@ -1794,10 +1794,10 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G3" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s" s="2">
         <v>34</v>
@@ -1806,16 +1806,16 @@
         <v>34</v>
       </c>
       <c r="J3" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K3" t="s" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M3" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -1866,22 +1866,22 @@
         <v>34</v>
       </c>
       <c r="AF3" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AG3" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH3" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI3" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ3" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK3" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL3" t="s" s="2">
         <v>34</v>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" t="s" s="2">
@@ -1906,28 +1906,28 @@
         <v>35</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M4" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N4" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" t="s" s="2">
@@ -1977,22 +1977,22 @@
         <v>34</v>
       </c>
       <c r="AF4" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AG4" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH4" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI4" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ4" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK4" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL4" t="s" s="2">
         <v>34</v>
@@ -2003,10 +2003,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s" s="2">
@@ -2017,7 +2017,7 @@
         <v>35</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H5" t="s" s="2">
         <v>34</v>
@@ -2029,16 +2029,16 @@
         <v>34</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N5" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" t="s" s="2">
@@ -2064,13 +2064,13 @@
         <v>34</v>
       </c>
       <c r="X5" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y5" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z5" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA5" t="s" s="2">
         <v>34</v>
@@ -2088,22 +2088,22 @@
         <v>34</v>
       </c>
       <c r="AF5" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AG5" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH5" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI5" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL5" t="s" s="2">
         <v>34</v>
@@ -2114,21 +2114,21 @@
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s" s="2">
         <v>34</v>
@@ -2140,16 +2140,16 @@
         <v>34</v>
       </c>
       <c r="K6" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L6" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N6" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" t="s" s="2">
@@ -2199,22 +2199,22 @@
         <v>34</v>
       </c>
       <c r="AF6" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AG6" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH6" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ6" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK6" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AL6" t="s" s="2">
         <v>34</v>
@@ -2225,14 +2225,14 @@
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" t="s" s="2">
@@ -2251,16 +2251,16 @@
         <v>34</v>
       </c>
       <c r="K7" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M7" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N7" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" t="s" s="2">
@@ -2310,7 +2310,7 @@
         <v>34</v>
       </c>
       <c r="AF7" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AG7" t="s" s="2">
         <v>35</v>
@@ -2325,7 +2325,7 @@
         <v>34</v>
       </c>
       <c r="AK7" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL7" t="s" s="2">
         <v>34</v>
@@ -2336,14 +2336,14 @@
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" t="s" s="2">
@@ -2362,16 +2362,16 @@
         <v>34</v>
       </c>
       <c r="K8" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L8" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M8" t="s" s="2">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="N8" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" t="s" s="2">
@@ -2409,19 +2409,19 @@
         <v>34</v>
       </c>
       <c r="AB8" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC8" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD8" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE8" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF8" t="s" s="2">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AG8" t="s" s="2">
         <v>35</v>
@@ -2430,13 +2430,13 @@
         <v>36</v>
       </c>
       <c r="AI8" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ8" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK8" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL8" t="s" s="2">
         <v>34</v>
@@ -2447,14 +2447,14 @@
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" t="s" s="2">
@@ -2467,25 +2467,25 @@
         <v>34</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s" s="2">
         <v>34</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M9" t="s" s="2">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N9" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O9" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P9" t="s" s="2">
         <v>34</v>
@@ -2522,19 +2522,19 @@
         <v>34</v>
       </c>
       <c r="AB9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD9" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE9" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF9" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AG9" t="s" s="2">
         <v>35</v>
@@ -2543,13 +2543,13 @@
         <v>36</v>
       </c>
       <c r="AI9" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK9" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL9" t="s" s="2">
         <v>34</v>
@@ -2560,10 +2560,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" t="s" s="2">
@@ -2571,10 +2571,10 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s" s="2">
         <v>34</v>
@@ -2583,20 +2583,20 @@
         <v>34</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P10" t="s" s="2">
         <v>34</v>
@@ -2645,7 +2645,7 @@
         <v>34</v>
       </c>
       <c r="AF10" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AG10" t="s" s="2">
         <v>35</v>
@@ -2654,27 +2654,27 @@
         <v>36</v>
       </c>
       <c r="AI10" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK10" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
@@ -2685,100 +2685,100 @@
         <v>35</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K11" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="L11" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="N11" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="O11" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="P11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Q11" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="R11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="S11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="T11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="U11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="V11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="X11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Y11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="Z11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AA11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AB11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AC11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AD11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AE11" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AF11" t="s" s="2">
         <v>113</v>
       </c>
-      <c r="L11" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="M11" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>116</v>
-      </c>
-      <c r="O11" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="P11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="Q11" t="s" s="2">
-        <v>118</v>
-      </c>
-      <c r="R11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="S11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="T11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="U11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="V11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="W11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="X11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="Y11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="Z11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AA11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AB11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AC11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AD11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AE11" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="AF11" t="s" s="2">
-        <v>112</v>
-      </c>
       <c r="AG11" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK11" t="s" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AM11" t="s" s="2">
         <v>34</v>
@@ -2786,10 +2786,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -2797,10 +2797,10 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>34</v>
@@ -2809,22 +2809,22 @@
         <v>34</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O12" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P12" t="s" s="2">
         <v>34</v>
@@ -2873,36 +2873,36 @@
         <v>34</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="AG12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AL12" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -2910,7 +2910,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>36</v>
@@ -2922,22 +2922,22 @@
         <v>34</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>34</v>
@@ -2962,29 +2962,29 @@
         <v>34</v>
       </c>
       <c r="X13" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y13" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z13" t="s" s="2">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AA13" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>35</v>
@@ -2993,40 +2993,40 @@
         <v>36</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s" s="2">
         <v>34</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s" s="2">
         <v>34</v>
@@ -3035,22 +3035,22 @@
         <v>34</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N14" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O14" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P14" t="s" s="2">
         <v>34</v>
@@ -3075,13 +3075,13 @@
         <v>34</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>34</v>
@@ -3099,7 +3099,7 @@
         <v>34</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>35</v>
@@ -3108,27 +3108,27 @@
         <v>36</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3139,7 +3139,7 @@
         <v>35</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s" s="2">
         <v>34</v>
@@ -3151,13 +3151,13 @@
         <v>34</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -3208,13 +3208,13 @@
         <v>34</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH15" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI15" t="s" s="2">
         <v>34</v>
@@ -3223,7 +3223,7 @@
         <v>34</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>34</v>
@@ -3234,14 +3234,14 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3260,16 +3260,16 @@
         <v>34</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" t="s" s="2">
@@ -3307,19 +3307,19 @@
         <v>34</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC16" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD16" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>35</v>
@@ -3328,13 +3328,13 @@
         <v>36</v>
       </c>
       <c r="AI16" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL16" t="s" s="2">
         <v>34</v>
@@ -3345,10 +3345,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3368,22 +3368,22 @@
         <v>34</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>34</v>
@@ -3432,7 +3432,7 @@
         <v>34</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>35</v>
@@ -3441,27 +3441,27 @@
         <v>36</v>
       </c>
       <c r="AI17" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3472,7 +3472,7 @@
         <v>35</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>34</v>
@@ -3484,13 +3484,13 @@
         <v>34</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
@@ -3541,13 +3541,13 @@
         <v>34</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>34</v>
@@ -3556,7 +3556,7 @@
         <v>34</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>34</v>
@@ -3567,14 +3567,14 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" t="s" s="2">
@@ -3593,16 +3593,16 @@
         <v>34</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -3640,19 +3640,19 @@
         <v>34</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC19" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD19" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>35</v>
@@ -3661,13 +3661,13 @@
         <v>36</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>34</v>
@@ -3678,10 +3678,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3692,7 +3692,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>34</v>
@@ -3701,29 +3701,29 @@
         <v>34</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>34</v>
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="S20" t="s" s="2">
         <v>34</v>
@@ -3765,36 +3765,36 @@
         <v>34</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH20" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI20" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3805,7 +3805,7 @@
         <v>35</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s" s="2">
         <v>34</v>
@@ -3814,19 +3814,19 @@
         <v>34</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -3876,36 +3876,36 @@
         <v>34</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH21" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI21" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AL21" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3916,7 +3916,7 @@
         <v>35</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>34</v>
@@ -3925,22 +3925,22 @@
         <v>34</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O22" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>34</v>
@@ -3989,36 +3989,36 @@
         <v>34</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI22" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4029,7 +4029,7 @@
         <v>35</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H23" t="s" s="2">
         <v>34</v>
@@ -4038,22 +4038,22 @@
         <v>34</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O23" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>34</v>
@@ -4102,36 +4102,36 @@
         <v>34</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4142,7 +4142,7 @@
         <v>35</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H24" t="s" s="2">
         <v>34</v>
@@ -4151,22 +4151,22 @@
         <v>34</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O24" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>34</v>
@@ -4215,36 +4215,36 @@
         <v>34</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4255,7 +4255,7 @@
         <v>35</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H25" t="s" s="2">
         <v>34</v>
@@ -4264,22 +4264,22 @@
         <v>34</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>34</v>
@@ -4328,36 +4328,36 @@
         <v>34</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI25" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C26" t="s" s="2">
         <v>27</v>
@@ -4366,13 +4366,13 @@
         <v>34</v>
       </c>
       <c r="E26" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>34</v>
@@ -4381,22 +4381,22 @@
         <v>34</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>34</v>
@@ -4421,13 +4421,13 @@
         <v>34</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="Z26" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>34</v>
@@ -4445,7 +4445,7 @@
         <v>34</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>35</v>
@@ -4454,27 +4454,27 @@
         <v>36</v>
       </c>
       <c r="AI26" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4485,7 +4485,7 @@
         <v>35</v>
       </c>
       <c r="G27" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H27" t="s" s="2">
         <v>34</v>
@@ -4497,13 +4497,13 @@
         <v>34</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4554,13 +4554,13 @@
         <v>34</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>34</v>
@@ -4569,7 +4569,7 @@
         <v>34</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>34</v>
@@ -4580,14 +4580,14 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -4606,16 +4606,16 @@
         <v>34</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4653,19 +4653,19 @@
         <v>34</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD28" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>35</v>
@@ -4674,13 +4674,13 @@
         <v>36</v>
       </c>
       <c r="AI28" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>34</v>
@@ -4691,10 +4691,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4714,22 +4714,22 @@
         <v>34</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>34</v>
@@ -4778,7 +4778,7 @@
         <v>34</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>35</v>
@@ -4787,27 +4787,27 @@
         <v>36</v>
       </c>
       <c r="AI29" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4818,7 +4818,7 @@
         <v>35</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>34</v>
@@ -4830,13 +4830,13 @@
         <v>34</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4887,13 +4887,13 @@
         <v>34</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH30" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI30" t="s" s="2">
         <v>34</v>
@@ -4902,7 +4902,7 @@
         <v>34</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>34</v>
@@ -4913,14 +4913,14 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -4939,16 +4939,16 @@
         <v>34</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" t="s" s="2">
@@ -4986,19 +4986,19 @@
         <v>34</v>
       </c>
       <c r="AB31" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC31" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD31" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>35</v>
@@ -5007,13 +5007,13 @@
         <v>36</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>34</v>
@@ -5024,10 +5024,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5038,7 +5038,7 @@
         <v>35</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>34</v>
@@ -5047,29 +5047,29 @@
         <v>34</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>34</v>
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="S32" t="s" s="2">
         <v>34</v>
@@ -5111,36 +5111,36 @@
         <v>34</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AL32" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5151,7 +5151,7 @@
         <v>35</v>
       </c>
       <c r="G33" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H33" t="s" s="2">
         <v>34</v>
@@ -5160,19 +5160,19 @@
         <v>34</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5222,36 +5222,36 @@
         <v>34</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH33" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AL33" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5262,7 +5262,7 @@
         <v>35</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>34</v>
@@ -5271,22 +5271,22 @@
         <v>34</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>34</v>
@@ -5335,36 +5335,36 @@
         <v>34</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH34" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AL34" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5375,7 +5375,7 @@
         <v>35</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>34</v>
@@ -5384,22 +5384,22 @@
         <v>34</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>34</v>
@@ -5448,36 +5448,36 @@
         <v>34</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AL35" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5488,7 +5488,7 @@
         <v>35</v>
       </c>
       <c r="G36" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H36" t="s" s="2">
         <v>34</v>
@@ -5497,22 +5497,22 @@
         <v>34</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="O36" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>34</v>
@@ -5561,36 +5561,36 @@
         <v>34</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AL36" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5601,7 +5601,7 @@
         <v>35</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>34</v>
@@ -5610,22 +5610,22 @@
         <v>34</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>34</v>
@@ -5674,36 +5674,36 @@
         <v>34</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AL37" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5711,10 +5711,10 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>34</v>
@@ -5723,22 +5723,22 @@
         <v>34</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>34</v>
@@ -5787,7 +5787,7 @@
         <v>34</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>35</v>
@@ -5796,27 +5796,27 @@
         <v>36</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AL38" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5827,7 +5827,7 @@
         <v>35</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>34</v>
@@ -5839,13 +5839,13 @@
         <v>34</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5896,13 +5896,13 @@
         <v>34</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>34</v>
@@ -5911,7 +5911,7 @@
         <v>34</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>34</v>
@@ -5922,14 +5922,14 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -5948,16 +5948,16 @@
         <v>34</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -5995,19 +5995,19 @@
         <v>34</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC40" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD40" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>35</v>
@@ -6016,13 +6016,13 @@
         <v>36</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>34</v>
@@ -6033,23 +6033,23 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="B41" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="B41" t="s" s="2">
-        <v>247</v>
-      </c>
       <c r="C41" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>34</v>
@@ -6061,16 +6061,16 @@
         <v>34</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6120,7 +6120,7 @@
         <v>34</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>35</v>
@@ -6129,13 +6129,13 @@
         <v>36</v>
       </c>
       <c r="AI41" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ41" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>34</v>
@@ -6146,10 +6146,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6160,31 +6160,31 @@
         <v>35</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>34</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>34</v>
@@ -6209,13 +6209,13 @@
         <v>34</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>34</v>
@@ -6233,36 +6233,36 @@
         <v>34</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6273,7 +6273,7 @@
         <v>35</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>34</v>
@@ -6282,22 +6282,22 @@
         <v>34</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>34</v>
@@ -6346,47 +6346,47 @@
         <v>34</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>34</v>
@@ -6395,19 +6395,19 @@
         <v>34</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6457,47 +6457,47 @@
         <v>34</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>34</v>
@@ -6506,19 +6506,19 @@
         <v>34</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6568,7 +6568,7 @@
         <v>34</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>35</v>
@@ -6577,27 +6577,27 @@
         <v>36</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6608,7 +6608,7 @@
         <v>35</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>34</v>
@@ -6617,19 +6617,19 @@
         <v>34</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -6655,13 +6655,13 @@
         <v>34</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>34</v>
@@ -6679,7 +6679,7 @@
         <v>34</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>35</v>
@@ -6688,27 +6688,27 @@
         <v>36</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AL46" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6728,19 +6728,19 @@
         <v>34</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6766,13 +6766,13 @@
         <v>34</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>34</v>
@@ -6790,7 +6790,7 @@
         <v>34</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>35</v>
@@ -6799,27 +6799,27 @@
         <v>36</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AL47" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6830,7 +6830,7 @@
         <v>35</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>34</v>
@@ -6839,22 +6839,22 @@
         <v>34</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>34</v>
@@ -6903,36 +6903,36 @@
         <v>34</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -6940,7 +6940,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>36</v>
@@ -6952,22 +6952,22 @@
         <v>34</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>34</v>
@@ -7016,7 +7016,7 @@
         <v>34</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>35</v>
@@ -7025,27 +7025,27 @@
         <v>36</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7056,7 +7056,7 @@
         <v>35</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>34</v>
@@ -7065,22 +7065,22 @@
         <v>34</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O50" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>34</v>
@@ -7105,13 +7105,13 @@
         <v>34</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>34</v>
@@ -7129,36 +7129,36 @@
         <v>34</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7169,7 +7169,7 @@
         <v>35</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>34</v>
@@ -7178,16 +7178,16 @@
         <v>34</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7238,22 +7238,22 @@
         <v>34</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>34</v>
@@ -7264,10 +7264,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7287,22 +7287,22 @@
         <v>34</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O52" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="P52" t="s" s="2">
         <v>34</v>
@@ -7351,7 +7351,7 @@
         <v>34</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>35</v>
@@ -7360,27 +7360,27 @@
         <v>36</v>
       </c>
       <c r="AI52" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7403,19 +7403,19 @@
         <v>34</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="O53" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="P53" t="s" s="2">
         <v>34</v>
@@ -7464,7 +7464,7 @@
         <v>34</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>35</v>
@@ -7473,27 +7473,27 @@
         <v>36</v>
       </c>
       <c r="AI53" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ53" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7504,7 +7504,7 @@
         <v>35</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>34</v>
@@ -7516,16 +7516,16 @@
         <v>34</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>357</v>
+        <v>310</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -7575,19 +7575,19 @@
         <v>34</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI54" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="AK54" t="s" s="2">
         <v>358</v>
@@ -7697,10 +7697,10 @@
         <v>36</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK55" t="s" s="2">
         <v>367</v>
@@ -7728,7 +7728,7 @@
         <v>35</v>
       </c>
       <c r="G56" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H56" t="s" s="2">
         <v>34</v>
@@ -7740,13 +7740,13 @@
         <v>34</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -7797,13 +7797,13 @@
         <v>34</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH56" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI56" t="s" s="2">
         <v>34</v>
@@ -7812,7 +7812,7 @@
         <v>34</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>34</v>
@@ -7830,7 +7830,7 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -7849,16 +7849,16 @@
         <v>34</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -7896,19 +7896,19 @@
         <v>34</v>
       </c>
       <c r="AB57" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AC57" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AD57" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>35</v>
@@ -7917,13 +7917,13 @@
         <v>36</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ57" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>34</v>
@@ -7954,13 +7954,13 @@
         <v>34</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J58" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L58" t="s" s="2">
         <v>372</v>
@@ -7969,10 +7969,10 @@
         <v>373</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O58" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>34</v>
@@ -8030,13 +8030,13 @@
         <v>36</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>34</v>
@@ -8058,10 +8058,10 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>34</v>
@@ -8073,7 +8073,7 @@
         <v>34</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="L59" t="s" s="2">
         <v>376</v>
@@ -8110,13 +8110,13 @@
         <v>34</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>34</v>
@@ -8137,16 +8137,16 @@
         <v>375</v>
       </c>
       <c r="AG59" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>380</v>
@@ -8174,7 +8174,7 @@
         <v>35</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>34</v>
@@ -8186,7 +8186,7 @@
         <v>34</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="L60" t="s" s="2">
         <v>383</v>
@@ -8253,13 +8253,13 @@
         <v>35</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>387</v>

</xml_diff>